<commit_message>
Next Step of Features Added. Pickling and unpickling successfully employed. Can update row data or alter threhsold. Merged .save_workbook() and .save_pickle() to .save().
</commit_message>
<xml_diff>
--- a/bucket_hat.xlsx
+++ b/bucket_hat.xlsx
@@ -414,13 +414,16 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="20" customWidth="1" min="1" max="1"/>
+  </cols>
   <sheetData>
     <row r="1">
       <c r="B1" t="inlineStr">
@@ -445,16 +448,30 @@
           <t>Threshold</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr">
+      <c r="B2" t="n">
+        <v>13.98</v>
+      </c>
+      <c r="C2" t="n">
+        <v>0.0003301233676692334</v>
+      </c>
+      <c r="D2" t="n">
+        <v>0.00468879702841619</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
         <is>
-          <t>13.98</t>
+          <t>23 Mar 22, 13:58PM</t>
         </is>
       </c>
-      <c r="C2" t="n">
-        <v>0.0003293172567778286</v>
-      </c>
-      <c r="D2" t="n">
-        <v>0.004696247201315487</v>
+      <c r="B3" t="n">
+        <v>13.98</v>
+      </c>
+      <c r="C3" t="n">
+        <v>0.0003301233676692334</v>
+      </c>
+      <c r="D3" t="n">
+        <v>0.00468879702841619</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Pickle and Openpyxl Resolved. Openpyxl data will no longer be stored in pickled object. Instead, all data will be solely stored in Excel document.
</commit_message>
<xml_diff>
--- a/bucket_hat.xlsx
+++ b/bucket_hat.xlsx
@@ -414,7 +414,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -422,7 +422,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="20" customWidth="1" min="1" max="1"/>
+    <col width="17" customWidth="1" min="1" max="1"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -452,26 +452,58 @@
         <v>13.98</v>
       </c>
       <c r="C2" t="n">
-        <v>0.0003301233676692334</v>
+        <v>0.0003182827846920551</v>
       </c>
       <c r="D2" t="n">
-        <v>0.00468879702841619</v>
+        <v>0.004508441233855234</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>23 Mar 22, 13:58PM</t>
+          <t>24 Mar 22, 17:37PM</t>
         </is>
       </c>
       <c r="B3" t="n">
         <v>13.98</v>
       </c>
       <c r="C3" t="n">
-        <v>0.0003301233676692334</v>
+        <v>0.0003182880746132817</v>
       </c>
       <c r="D3" t="n">
-        <v>0.00468879702841619</v>
+        <v>0.004509815623382007</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>24 Mar 22, 17:37PM</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>13.98</v>
+      </c>
+      <c r="C4" t="n">
+        <v>0.0003182880746132817</v>
+      </c>
+      <c r="D4" t="n">
+        <v>0.004509815623382007</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>24 Mar 22, 17:37PM</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>13.98</v>
+      </c>
+      <c r="C5" t="n">
+        <v>0.0003181687680484818</v>
+      </c>
+      <c r="D5" t="n">
+        <v>0.004509815623382007</v>
       </c>
     </row>
   </sheetData>

</xml_diff>